<commit_message>
atualização arquivos e target
no target - introdução dos gráficos de plds anuais, horarios, etc.
</commit_message>
<xml_diff>
--- a/assets/testepld.xlsx
+++ b/assets/testepld.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1466"/>
+  <dimension ref="A1:E1474"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28295,6 +28295,158 @@
         <v>61.06999999999999</v>
       </c>
     </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>05/01/2024</t>
+        </is>
+      </c>
+      <c r="B1467" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="C1467" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="D1467" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="E1467" t="n">
+        <v>61.06999999999999</v>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>06/01/2024</t>
+        </is>
+      </c>
+      <c r="B1468" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="C1468" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="D1468" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="E1468" t="n">
+        <v>61.06999999999999</v>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>07/01/2024</t>
+        </is>
+      </c>
+      <c r="B1469" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="C1469" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="D1469" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="E1469" t="n">
+        <v>61.06999999999999</v>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>08/01/2024</t>
+        </is>
+      </c>
+      <c r="B1470" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="C1470" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="D1470" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="E1470" t="n">
+        <v>61.06999999999999</v>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>09/01/2024</t>
+        </is>
+      </c>
+      <c r="B1471" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="C1471" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="D1471" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="E1471" t="n">
+        <v>61.06999999999999</v>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>10/01/2024</t>
+        </is>
+      </c>
+      <c r="B1472" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="C1472" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="D1472" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="E1472" t="n">
+        <v>61.06999999999999</v>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>11/01/2024</t>
+        </is>
+      </c>
+      <c r="B1473" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="C1473" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="D1473" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="E1473" t="n">
+        <v>61.06999999999999</v>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>12/01/2024</t>
+        </is>
+      </c>
+      <c r="B1474" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="C1474" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="D1474" t="n">
+        <v>61.06999999999999</v>
+      </c>
+      <c r="E1474" t="n">
+        <v>61.06999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>